<commit_message>
Complete all error free response
</commit_message>
<xml_diff>
--- a/check.xlsx
+++ b/check.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\TimetableInternship\timetable_python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29EE0A5E-BE6D-4177-8409-43D7AD4F26D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20F6B24C-D0C7-4AB7-ABE8-8877FE6CE878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Time/Day</t>
   </si>
@@ -84,6 +84,9 @@
     <t>(("PSOT", "L","B505","RBS","B1"),
 ("PSOT", "L","CCF","JVJ","B2"),
 ("PSOT", "L","B215","VPV","B3"))</t>
+  </si>
+  <si>
+    <t>("PSOT","L","B505","RBS","B1")</t>
   </si>
 </sst>
 </file>
@@ -407,7 +410,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -463,6 +466,9 @@
       <c r="C4" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">

</xml_diff>